<commit_message>
Updated data set and moment-based classification
</commit_message>
<xml_diff>
--- a/documentation/simulation_runs_v05202024.xlsx
+++ b/documentation/simulation_runs_v05202024.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Slava\Documents\kineticsim_reader\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2D5E55E-4E91-4E88-A8E3-C9D1082A951E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A5A8D66-C221-4458-935D-9002611D075E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="840" yWindow="3015" windowWidth="34215" windowHeight="15435" xr2:uid="{D37B92F4-10C5-452F-896A-B11031BDCD63}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{D37B92F4-10C5-452F-896A-B11031BDCD63}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Summary of the runs" sheetId="1" r:id="rId1"/>
+    <sheet name="exp1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="148">
   <si>
     <t>particles.d11_A0.5Hepp_beta0.5eps1e-4_256</t>
   </si>
@@ -503,7 +504,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -513,6 +514,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -529,7 +536,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -549,6 +556,14 @@
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -885,9 +900,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36FA8923-3A61-45EC-9C7E-795683E14795}">
   <dimension ref="A2:AC25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D14" sqref="D14"/>
+      <selection pane="topRight" activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3045,4 +3060,2170 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A84B8E6-5357-4041-9260-018E6244495A}">
+  <dimension ref="A2:AC25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="K24" sqref="K24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="65.85546875" customWidth="1"/>
+    <col min="2" max="2" width="62.42578125" customWidth="1"/>
+    <col min="3" max="3" width="64.140625" customWidth="1"/>
+    <col min="4" max="4" width="31" customWidth="1"/>
+    <col min="5" max="5" width="31" style="2" customWidth="1"/>
+    <col min="6" max="6" width="37.7109375" customWidth="1"/>
+    <col min="7" max="7" width="18.7109375" customWidth="1"/>
+    <col min="8" max="8" width="22" customWidth="1"/>
+    <col min="9" max="9" width="25.7109375" customWidth="1"/>
+    <col min="18" max="18" width="12.28515625" customWidth="1"/>
+    <col min="29" max="29" width="11.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="E3" s="7">
+        <v>0</v>
+      </c>
+      <c r="F3" t="s">
+        <v>97</v>
+      </c>
+      <c r="G3" t="s">
+        <v>98</v>
+      </c>
+      <c r="H3" t="s">
+        <v>99</v>
+      </c>
+      <c r="I3" t="s">
+        <v>100</v>
+      </c>
+      <c r="J3">
+        <v>1.5</v>
+      </c>
+      <c r="K3">
+        <v>1.5</v>
+      </c>
+      <c r="L3">
+        <v>0.05</v>
+      </c>
+      <c r="M3">
+        <v>1000.1</v>
+      </c>
+      <c r="N3" s="3">
+        <v>10000</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>0.5</v>
+      </c>
+      <c r="Q3" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="R3" t="s">
+        <v>101</v>
+      </c>
+      <c r="S3">
+        <v>0</v>
+      </c>
+      <c r="T3">
+        <v>50</v>
+      </c>
+      <c r="U3">
+        <v>250</v>
+      </c>
+      <c r="V3">
+        <v>50</v>
+      </c>
+      <c r="W3">
+        <v>500</v>
+      </c>
+      <c r="X3">
+        <v>0</v>
+      </c>
+      <c r="Y3">
+        <v>0</v>
+      </c>
+      <c r="Z3">
+        <v>0.04</v>
+      </c>
+      <c r="AA3">
+        <v>0.42</v>
+      </c>
+      <c r="AB3">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="AC3" s="3">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="E4" s="7">
+        <v>0</v>
+      </c>
+      <c r="F4" t="s">
+        <v>97</v>
+      </c>
+      <c r="G4" t="s">
+        <v>102</v>
+      </c>
+      <c r="H4" t="s">
+        <v>99</v>
+      </c>
+      <c r="I4" t="s">
+        <v>103</v>
+      </c>
+      <c r="J4">
+        <v>1.5</v>
+      </c>
+      <c r="K4">
+        <v>1.5</v>
+      </c>
+      <c r="L4">
+        <v>0.05</v>
+      </c>
+      <c r="M4">
+        <v>610.1</v>
+      </c>
+      <c r="N4" s="3">
+        <v>10000</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="R4" t="s">
+        <v>101</v>
+      </c>
+      <c r="S4">
+        <v>0</v>
+      </c>
+      <c r="T4">
+        <v>50</v>
+      </c>
+      <c r="U4">
+        <v>250</v>
+      </c>
+      <c r="V4">
+        <v>50</v>
+      </c>
+      <c r="W4">
+        <v>500</v>
+      </c>
+      <c r="X4">
+        <v>0</v>
+      </c>
+      <c r="Y4">
+        <v>0</v>
+      </c>
+      <c r="Z4">
+        <v>0.04</v>
+      </c>
+      <c r="AA4">
+        <v>0.42</v>
+      </c>
+      <c r="AB4">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="AC4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="E5" s="10">
+        <v>0.42</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="I5" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="J5" s="11">
+        <v>0.75</v>
+      </c>
+      <c r="K5" s="11">
+        <v>0.75</v>
+      </c>
+      <c r="L5" s="11">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="M5" s="11">
+        <v>600.1</v>
+      </c>
+      <c r="N5" s="12">
+        <v>10000</v>
+      </c>
+      <c r="O5" s="11">
+        <v>0</v>
+      </c>
+      <c r="P5" s="11">
+        <v>0.08</v>
+      </c>
+      <c r="Q5" s="12">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="R5" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="S5" s="11">
+        <v>0</v>
+      </c>
+      <c r="T5" s="11">
+        <v>50</v>
+      </c>
+      <c r="U5" s="11">
+        <v>500</v>
+      </c>
+      <c r="V5" s="11">
+        <v>50</v>
+      </c>
+      <c r="W5" s="11">
+        <v>500</v>
+      </c>
+      <c r="X5" s="11">
+        <v>0</v>
+      </c>
+      <c r="Y5" s="11">
+        <v>0</v>
+      </c>
+      <c r="Z5" s="11">
+        <v>0.04</v>
+      </c>
+      <c r="AA5" s="11">
+        <v>0.42</v>
+      </c>
+      <c r="AB5" s="11">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="AC5" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="E6" s="7">
+        <v>0</v>
+      </c>
+      <c r="F6" t="s">
+        <v>97</v>
+      </c>
+      <c r="G6" t="s">
+        <v>108</v>
+      </c>
+      <c r="H6" t="s">
+        <v>106</v>
+      </c>
+      <c r="I6" t="s">
+        <v>107</v>
+      </c>
+      <c r="J6">
+        <v>0.75</v>
+      </c>
+      <c r="K6">
+        <v>0.75</v>
+      </c>
+      <c r="L6">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="M6">
+        <v>600.1</v>
+      </c>
+      <c r="N6" s="3">
+        <v>10000</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <v>0.08</v>
+      </c>
+      <c r="Q6" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="R6" t="s">
+        <v>101</v>
+      </c>
+      <c r="S6">
+        <v>0</v>
+      </c>
+      <c r="T6">
+        <v>50</v>
+      </c>
+      <c r="U6">
+        <v>500</v>
+      </c>
+      <c r="V6">
+        <v>50</v>
+      </c>
+      <c r="W6">
+        <v>500</v>
+      </c>
+      <c r="X6">
+        <v>0</v>
+      </c>
+      <c r="Y6">
+        <v>0</v>
+      </c>
+      <c r="Z6">
+        <v>0.04</v>
+      </c>
+      <c r="AA6">
+        <v>0.42</v>
+      </c>
+      <c r="AB6">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="AC6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="E7" s="7">
+        <v>0.32</v>
+      </c>
+      <c r="F7" t="s">
+        <v>109</v>
+      </c>
+      <c r="G7" t="s">
+        <v>108</v>
+      </c>
+      <c r="H7" t="s">
+        <v>106</v>
+      </c>
+      <c r="I7" t="s">
+        <v>107</v>
+      </c>
+      <c r="J7">
+        <v>0.75</v>
+      </c>
+      <c r="K7">
+        <v>0.75</v>
+      </c>
+      <c r="L7">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="M7">
+        <v>600.1</v>
+      </c>
+      <c r="N7" s="3">
+        <v>10000</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>0.08</v>
+      </c>
+      <c r="Q7" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="R7" t="s">
+        <v>101</v>
+      </c>
+      <c r="S7">
+        <v>0</v>
+      </c>
+      <c r="T7">
+        <v>50</v>
+      </c>
+      <c r="U7">
+        <v>500</v>
+      </c>
+      <c r="V7">
+        <v>50</v>
+      </c>
+      <c r="W7">
+        <v>500</v>
+      </c>
+      <c r="X7">
+        <v>0</v>
+      </c>
+      <c r="Y7">
+        <v>0</v>
+      </c>
+      <c r="Z7">
+        <v>0.04</v>
+      </c>
+      <c r="AA7">
+        <v>0.42</v>
+      </c>
+      <c r="AB7">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="AC7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="E8" s="7">
+        <v>0.32</v>
+      </c>
+      <c r="F8" t="s">
+        <v>109</v>
+      </c>
+      <c r="G8" t="s">
+        <v>110</v>
+      </c>
+      <c r="H8" t="s">
+        <v>106</v>
+      </c>
+      <c r="I8" t="s">
+        <v>111</v>
+      </c>
+      <c r="J8">
+        <v>0.75</v>
+      </c>
+      <c r="K8">
+        <v>0.75</v>
+      </c>
+      <c r="L8">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="M8">
+        <v>5000.1000000000004</v>
+      </c>
+      <c r="N8" s="3">
+        <v>10000</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
+      </c>
+      <c r="P8">
+        <v>0.1</v>
+      </c>
+      <c r="Q8" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="R8" t="s">
+        <v>101</v>
+      </c>
+      <c r="S8">
+        <v>0</v>
+      </c>
+      <c r="T8">
+        <v>100</v>
+      </c>
+      <c r="U8">
+        <v>8000</v>
+      </c>
+      <c r="V8">
+        <v>100</v>
+      </c>
+      <c r="W8">
+        <v>1000</v>
+      </c>
+      <c r="X8">
+        <v>0</v>
+      </c>
+      <c r="Y8">
+        <v>0</v>
+      </c>
+      <c r="Z8">
+        <v>0.04</v>
+      </c>
+      <c r="AA8">
+        <v>0.42</v>
+      </c>
+      <c r="AB8">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="AC8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="E9" s="7">
+        <v>0.32</v>
+      </c>
+      <c r="F9" t="s">
+        <v>109</v>
+      </c>
+      <c r="G9" t="s">
+        <v>110</v>
+      </c>
+      <c r="H9" t="s">
+        <v>106</v>
+      </c>
+      <c r="I9" t="s">
+        <v>111</v>
+      </c>
+      <c r="J9">
+        <v>0.75</v>
+      </c>
+      <c r="K9">
+        <v>0.75</v>
+      </c>
+      <c r="L9">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="M9">
+        <v>5000.1000000000004</v>
+      </c>
+      <c r="N9" s="3">
+        <v>10000</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+      <c r="P9">
+        <v>0.1</v>
+      </c>
+      <c r="Q9" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="R9" t="s">
+        <v>101</v>
+      </c>
+      <c r="S9">
+        <v>0</v>
+      </c>
+      <c r="T9">
+        <v>100</v>
+      </c>
+      <c r="U9">
+        <v>4000</v>
+      </c>
+      <c r="V9">
+        <v>100</v>
+      </c>
+      <c r="W9">
+        <v>1000</v>
+      </c>
+      <c r="X9">
+        <v>0</v>
+      </c>
+      <c r="Y9">
+        <v>0</v>
+      </c>
+      <c r="Z9">
+        <v>0.04</v>
+      </c>
+      <c r="AA9">
+        <v>0.42</v>
+      </c>
+      <c r="AB9">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="AC9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="E10" s="7">
+        <v>0</v>
+      </c>
+      <c r="F10" t="s">
+        <v>97</v>
+      </c>
+      <c r="G10" t="s">
+        <v>112</v>
+      </c>
+      <c r="H10" t="s">
+        <v>99</v>
+      </c>
+      <c r="I10" t="s">
+        <v>113</v>
+      </c>
+      <c r="J10">
+        <v>0.75</v>
+      </c>
+      <c r="K10">
+        <v>0.75</v>
+      </c>
+      <c r="L10">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="M10">
+        <v>600.1</v>
+      </c>
+      <c r="N10" s="3">
+        <v>10000</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
+      <c r="P10">
+        <v>2.0670000000000001E-2</v>
+      </c>
+      <c r="Q10" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="R10" t="s">
+        <v>101</v>
+      </c>
+      <c r="S10">
+        <v>0</v>
+      </c>
+      <c r="T10">
+        <v>50</v>
+      </c>
+      <c r="U10">
+        <v>500</v>
+      </c>
+      <c r="V10">
+        <v>50</v>
+      </c>
+      <c r="W10">
+        <v>500</v>
+      </c>
+      <c r="X10">
+        <v>0</v>
+      </c>
+      <c r="Y10">
+        <v>0</v>
+      </c>
+      <c r="Z10">
+        <v>0.04</v>
+      </c>
+      <c r="AA10">
+        <v>0.42</v>
+      </c>
+      <c r="AB10">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="AC10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:29" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="E11" s="8">
+        <v>2</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="J11" s="5">
+        <v>0.75</v>
+      </c>
+      <c r="K11" s="5">
+        <v>0.75</v>
+      </c>
+      <c r="L11" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="M11" s="5">
+        <v>200.1</v>
+      </c>
+      <c r="N11" s="6">
+        <v>10000</v>
+      </c>
+      <c r="O11" s="5">
+        <v>0</v>
+      </c>
+      <c r="P11" s="5">
+        <v>2.0670000000000001E-2</v>
+      </c>
+      <c r="Q11" s="6">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="R11" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="S11" s="5">
+        <v>0</v>
+      </c>
+      <c r="T11" s="5">
+        <v>20</v>
+      </c>
+      <c r="U11" s="5">
+        <v>800</v>
+      </c>
+      <c r="V11" s="5">
+        <v>50</v>
+      </c>
+      <c r="W11" s="5">
+        <v>1250</v>
+      </c>
+      <c r="X11" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y11" s="5">
+        <v>0</v>
+      </c>
+      <c r="Z11" s="5">
+        <v>0.04</v>
+      </c>
+      <c r="AA11" s="5">
+        <v>0.42</v>
+      </c>
+      <c r="AB11" s="5">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="AC11" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:29" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="E12" s="10">
+        <v>2</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="H12" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="I12" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="J12" s="11">
+        <v>0.75</v>
+      </c>
+      <c r="K12" s="11">
+        <v>0.75</v>
+      </c>
+      <c r="L12" s="11">
+        <v>0.01</v>
+      </c>
+      <c r="M12" s="11">
+        <v>600.1</v>
+      </c>
+      <c r="N12" s="12">
+        <v>10000</v>
+      </c>
+      <c r="O12" s="11">
+        <v>0</v>
+      </c>
+      <c r="P12" s="11">
+        <v>2.0670000000000001E-2</v>
+      </c>
+      <c r="Q12" s="12">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="R12" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="S12" s="11">
+        <v>0</v>
+      </c>
+      <c r="T12" s="11">
+        <v>50</v>
+      </c>
+      <c r="U12" s="11">
+        <v>650</v>
+      </c>
+      <c r="V12" s="11">
+        <v>50</v>
+      </c>
+      <c r="W12" s="11">
+        <v>1250</v>
+      </c>
+      <c r="X12" s="11">
+        <v>0</v>
+      </c>
+      <c r="Y12" s="11">
+        <v>0</v>
+      </c>
+      <c r="Z12" s="11">
+        <v>0.04</v>
+      </c>
+      <c r="AA12" s="11">
+        <v>0.42</v>
+      </c>
+      <c r="AB12" s="11">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="AC12" s="12">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:29" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="E13" s="10">
+        <v>1.5</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="H13" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="I13" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="J13" s="11">
+        <v>0.75</v>
+      </c>
+      <c r="K13" s="11">
+        <v>0.75</v>
+      </c>
+      <c r="L13" s="11">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="M13" s="11">
+        <v>1000.1</v>
+      </c>
+      <c r="N13" s="12">
+        <v>10000</v>
+      </c>
+      <c r="O13" s="11">
+        <v>0</v>
+      </c>
+      <c r="P13" s="11">
+        <v>2.0670000000000001E-2</v>
+      </c>
+      <c r="Q13" s="12">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="R13" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="S13" s="11">
+        <v>0</v>
+      </c>
+      <c r="T13" s="11">
+        <v>50</v>
+      </c>
+      <c r="U13" s="11">
+        <v>500</v>
+      </c>
+      <c r="V13" s="11">
+        <v>50</v>
+      </c>
+      <c r="W13" s="11">
+        <v>500</v>
+      </c>
+      <c r="X13" s="11">
+        <v>0</v>
+      </c>
+      <c r="Y13" s="11">
+        <v>0</v>
+      </c>
+      <c r="Z13" s="11">
+        <v>0.04</v>
+      </c>
+      <c r="AA13" s="11">
+        <v>0.42</v>
+      </c>
+      <c r="AB13" s="11">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="AC13" s="12">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="E14" s="7">
+        <v>0</v>
+      </c>
+      <c r="F14" t="s">
+        <v>115</v>
+      </c>
+      <c r="G14" t="s">
+        <v>103</v>
+      </c>
+      <c r="H14" t="s">
+        <v>116</v>
+      </c>
+      <c r="I14" t="s">
+        <v>117</v>
+      </c>
+      <c r="J14">
+        <v>0.75</v>
+      </c>
+      <c r="K14">
+        <v>0.75</v>
+      </c>
+      <c r="L14">
+        <v>0.02</v>
+      </c>
+      <c r="M14">
+        <v>3000.1</v>
+      </c>
+      <c r="N14" s="3">
+        <v>10000</v>
+      </c>
+      <c r="O14">
+        <v>0</v>
+      </c>
+      <c r="P14">
+        <v>4.1300000000000003E-2</v>
+      </c>
+      <c r="Q14" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="R14" t="s">
+        <v>101</v>
+      </c>
+      <c r="S14">
+        <v>0</v>
+      </c>
+      <c r="T14">
+        <v>50</v>
+      </c>
+      <c r="U14">
+        <v>1000</v>
+      </c>
+      <c r="V14">
+        <v>50</v>
+      </c>
+      <c r="W14">
+        <v>1250</v>
+      </c>
+      <c r="X14">
+        <v>0</v>
+      </c>
+      <c r="Y14">
+        <v>0</v>
+      </c>
+      <c r="Z14">
+        <v>0.04</v>
+      </c>
+      <c r="AA14">
+        <v>0.42</v>
+      </c>
+      <c r="AB14">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="AC14" s="3">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="E15" s="7">
+        <v>0</v>
+      </c>
+      <c r="F15" t="s">
+        <v>118</v>
+      </c>
+      <c r="G15" t="s">
+        <v>119</v>
+      </c>
+      <c r="H15" t="s">
+        <v>120</v>
+      </c>
+      <c r="I15" t="s">
+        <v>121</v>
+      </c>
+      <c r="J15">
+        <v>0.75</v>
+      </c>
+      <c r="K15">
+        <v>0.75</v>
+      </c>
+      <c r="L15">
+        <v>0.02</v>
+      </c>
+      <c r="M15">
+        <v>3000.1</v>
+      </c>
+      <c r="N15" s="3">
+        <v>10000</v>
+      </c>
+      <c r="O15">
+        <v>0</v>
+      </c>
+      <c r="P15">
+        <v>0.42899999999999999</v>
+      </c>
+      <c r="Q15" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="R15" t="s">
+        <v>101</v>
+      </c>
+      <c r="S15">
+        <v>0</v>
+      </c>
+      <c r="T15">
+        <v>50</v>
+      </c>
+      <c r="U15">
+        <v>2500</v>
+      </c>
+      <c r="V15">
+        <v>50</v>
+      </c>
+      <c r="W15">
+        <v>1250</v>
+      </c>
+      <c r="X15">
+        <v>0</v>
+      </c>
+      <c r="Y15">
+        <v>0</v>
+      </c>
+      <c r="Z15">
+        <v>0.04</v>
+      </c>
+      <c r="AA15">
+        <v>0.42</v>
+      </c>
+      <c r="AB15">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="AC15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="E16" s="7">
+        <v>0</v>
+      </c>
+      <c r="F16" t="s">
+        <v>122</v>
+      </c>
+      <c r="G16" t="s">
+        <v>123</v>
+      </c>
+      <c r="H16" t="s">
+        <v>124</v>
+      </c>
+      <c r="I16" t="s">
+        <v>125</v>
+      </c>
+      <c r="J16">
+        <v>0.75</v>
+      </c>
+      <c r="K16">
+        <v>0.75</v>
+      </c>
+      <c r="L16">
+        <v>0.02</v>
+      </c>
+      <c r="M16">
+        <v>3000.1</v>
+      </c>
+      <c r="N16" s="3">
+        <v>10000</v>
+      </c>
+      <c r="O16">
+        <v>0</v>
+      </c>
+      <c r="P16">
+        <v>0.42899999999999999</v>
+      </c>
+      <c r="Q16" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="R16" t="s">
+        <v>101</v>
+      </c>
+      <c r="S16">
+        <v>0</v>
+      </c>
+      <c r="T16">
+        <v>50</v>
+      </c>
+      <c r="U16">
+        <v>2000</v>
+      </c>
+      <c r="V16">
+        <v>50</v>
+      </c>
+      <c r="W16">
+        <v>1250</v>
+      </c>
+      <c r="X16">
+        <v>0</v>
+      </c>
+      <c r="Y16">
+        <v>0</v>
+      </c>
+      <c r="Z16">
+        <v>0.04</v>
+      </c>
+      <c r="AA16">
+        <v>0.42</v>
+      </c>
+      <c r="AB16">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="AC16" s="3">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="E17" s="7">
+        <v>0</v>
+      </c>
+      <c r="F17" t="s">
+        <v>126</v>
+      </c>
+      <c r="G17" t="s">
+        <v>103</v>
+      </c>
+      <c r="H17" t="s">
+        <v>120</v>
+      </c>
+      <c r="I17" t="s">
+        <v>127</v>
+      </c>
+      <c r="J17">
+        <v>0.75</v>
+      </c>
+      <c r="K17">
+        <v>0.75</v>
+      </c>
+      <c r="L17">
+        <v>0.02</v>
+      </c>
+      <c r="M17">
+        <v>3000.1</v>
+      </c>
+      <c r="N17" s="3">
+        <v>10000</v>
+      </c>
+      <c r="O17">
+        <v>0</v>
+      </c>
+      <c r="P17">
+        <v>0.42899999999999999</v>
+      </c>
+      <c r="Q17" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="R17" t="s">
+        <v>101</v>
+      </c>
+      <c r="S17">
+        <v>0</v>
+      </c>
+      <c r="T17">
+        <v>50</v>
+      </c>
+      <c r="U17">
+        <v>2500</v>
+      </c>
+      <c r="V17">
+        <v>50</v>
+      </c>
+      <c r="W17">
+        <v>1250</v>
+      </c>
+      <c r="X17">
+        <v>0</v>
+      </c>
+      <c r="Y17">
+        <v>0</v>
+      </c>
+      <c r="Z17">
+        <v>0.04</v>
+      </c>
+      <c r="AA17">
+        <v>0.42</v>
+      </c>
+      <c r="AB17">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="AC17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="E18" s="7">
+        <v>0</v>
+      </c>
+      <c r="F18" t="s">
+        <v>126</v>
+      </c>
+      <c r="G18" t="s">
+        <v>128</v>
+      </c>
+      <c r="H18" t="s">
+        <v>120</v>
+      </c>
+      <c r="I18" t="s">
+        <v>127</v>
+      </c>
+      <c r="J18">
+        <v>0.75</v>
+      </c>
+      <c r="K18">
+        <v>0.75</v>
+      </c>
+      <c r="L18">
+        <v>0.02</v>
+      </c>
+      <c r="M18">
+        <v>3000.1</v>
+      </c>
+      <c r="N18" s="3">
+        <v>10000</v>
+      </c>
+      <c r="O18">
+        <v>0</v>
+      </c>
+      <c r="P18">
+        <v>0.42899999999999999</v>
+      </c>
+      <c r="Q18" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="R18" t="s">
+        <v>101</v>
+      </c>
+      <c r="S18">
+        <v>0</v>
+      </c>
+      <c r="T18">
+        <v>50</v>
+      </c>
+      <c r="U18">
+        <v>2500</v>
+      </c>
+      <c r="V18">
+        <v>50</v>
+      </c>
+      <c r="W18">
+        <v>1250</v>
+      </c>
+      <c r="X18">
+        <v>0</v>
+      </c>
+      <c r="Y18">
+        <v>0</v>
+      </c>
+      <c r="Z18">
+        <v>0.04</v>
+      </c>
+      <c r="AA18">
+        <v>0.42</v>
+      </c>
+      <c r="AB18">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="AC18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="E19" s="7">
+        <v>0</v>
+      </c>
+      <c r="F19" t="s">
+        <v>126</v>
+      </c>
+      <c r="G19" t="s">
+        <v>119</v>
+      </c>
+      <c r="H19" t="s">
+        <v>120</v>
+      </c>
+      <c r="I19" t="s">
+        <v>121</v>
+      </c>
+      <c r="J19">
+        <v>0.75</v>
+      </c>
+      <c r="K19">
+        <v>0.75</v>
+      </c>
+      <c r="L19">
+        <v>0.02</v>
+      </c>
+      <c r="M19">
+        <v>3000.1</v>
+      </c>
+      <c r="N19" s="3">
+        <v>10000</v>
+      </c>
+      <c r="O19">
+        <v>0</v>
+      </c>
+      <c r="P19">
+        <v>0.42899999999999999</v>
+      </c>
+      <c r="Q19" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="R19" t="s">
+        <v>101</v>
+      </c>
+      <c r="S19">
+        <v>0</v>
+      </c>
+      <c r="T19">
+        <v>50</v>
+      </c>
+      <c r="U19">
+        <v>2500</v>
+      </c>
+      <c r="V19">
+        <v>50</v>
+      </c>
+      <c r="W19">
+        <v>1250</v>
+      </c>
+      <c r="X19">
+        <v>0</v>
+      </c>
+      <c r="Y19">
+        <v>0</v>
+      </c>
+      <c r="Z19">
+        <v>0.04</v>
+      </c>
+      <c r="AA19">
+        <v>0.42</v>
+      </c>
+      <c r="AB19">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="AC19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="E20" s="7">
+        <v>0</v>
+      </c>
+      <c r="F20" t="s">
+        <v>129</v>
+      </c>
+      <c r="G20" t="s">
+        <v>130</v>
+      </c>
+      <c r="H20" t="s">
+        <v>131</v>
+      </c>
+      <c r="I20" t="s">
+        <v>132</v>
+      </c>
+      <c r="J20">
+        <v>0.75</v>
+      </c>
+      <c r="K20">
+        <v>0.75</v>
+      </c>
+      <c r="L20">
+        <v>0.02</v>
+      </c>
+      <c r="M20">
+        <v>3000.1</v>
+      </c>
+      <c r="N20" s="3">
+        <v>10000</v>
+      </c>
+      <c r="O20">
+        <v>0</v>
+      </c>
+      <c r="P20">
+        <v>0.42899999999999999</v>
+      </c>
+      <c r="Q20" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="R20" t="s">
+        <v>101</v>
+      </c>
+      <c r="S20">
+        <v>0</v>
+      </c>
+      <c r="T20">
+        <v>50</v>
+      </c>
+      <c r="U20">
+        <v>2000</v>
+      </c>
+      <c r="V20">
+        <v>50</v>
+      </c>
+      <c r="W20">
+        <v>1250</v>
+      </c>
+      <c r="X20">
+        <v>0</v>
+      </c>
+      <c r="Y20">
+        <v>0</v>
+      </c>
+      <c r="Z20">
+        <v>0.04</v>
+      </c>
+      <c r="AA20">
+        <v>0.42</v>
+      </c>
+      <c r="AB20">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="AC20" s="3">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="E21" s="7">
+        <v>0</v>
+      </c>
+      <c r="F21" t="s">
+        <v>133</v>
+      </c>
+      <c r="G21" t="s">
+        <v>130</v>
+      </c>
+      <c r="H21" t="s">
+        <v>134</v>
+      </c>
+      <c r="I21" t="s">
+        <v>135</v>
+      </c>
+      <c r="J21">
+        <v>0.75</v>
+      </c>
+      <c r="K21">
+        <v>0.75</v>
+      </c>
+      <c r="L21">
+        <v>0.02</v>
+      </c>
+      <c r="M21">
+        <v>3000.1</v>
+      </c>
+      <c r="N21" s="3">
+        <v>10000</v>
+      </c>
+      <c r="O21">
+        <v>0</v>
+      </c>
+      <c r="P21">
+        <v>0.42899999999999999</v>
+      </c>
+      <c r="Q21" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="R21" t="s">
+        <v>101</v>
+      </c>
+      <c r="S21">
+        <v>0</v>
+      </c>
+      <c r="T21">
+        <v>50</v>
+      </c>
+      <c r="U21">
+        <v>2500</v>
+      </c>
+      <c r="V21">
+        <v>50</v>
+      </c>
+      <c r="W21">
+        <v>1250</v>
+      </c>
+      <c r="X21">
+        <v>0</v>
+      </c>
+      <c r="Y21">
+        <v>0</v>
+      </c>
+      <c r="Z21">
+        <v>0.04</v>
+      </c>
+      <c r="AA21">
+        <v>0.42</v>
+      </c>
+      <c r="AB21">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="AC21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="E22" s="7">
+        <v>0</v>
+      </c>
+      <c r="F22" t="s">
+        <v>136</v>
+      </c>
+      <c r="G22" t="s">
+        <v>130</v>
+      </c>
+      <c r="H22" t="s">
+        <v>137</v>
+      </c>
+      <c r="I22" t="s">
+        <v>132</v>
+      </c>
+      <c r="J22">
+        <v>0.75</v>
+      </c>
+      <c r="K22">
+        <v>0.75</v>
+      </c>
+      <c r="L22">
+        <v>0.02</v>
+      </c>
+      <c r="M22">
+        <v>6000.1</v>
+      </c>
+      <c r="N22" s="3">
+        <v>10000</v>
+      </c>
+      <c r="O22">
+        <v>0</v>
+      </c>
+      <c r="P22">
+        <v>0.42899999999999999</v>
+      </c>
+      <c r="Q22" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="R22" t="s">
+        <v>101</v>
+      </c>
+      <c r="S22">
+        <v>1</v>
+      </c>
+      <c r="T22">
+        <v>50</v>
+      </c>
+      <c r="U22">
+        <v>2000</v>
+      </c>
+      <c r="V22">
+        <v>50</v>
+      </c>
+      <c r="W22">
+        <v>1250</v>
+      </c>
+      <c r="X22">
+        <v>0</v>
+      </c>
+      <c r="Y22">
+        <v>0</v>
+      </c>
+      <c r="Z22">
+        <v>0.04</v>
+      </c>
+      <c r="AA22">
+        <v>0.42</v>
+      </c>
+      <c r="AB22">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="AC22" s="3">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="E23" s="7">
+        <v>1.2</v>
+      </c>
+      <c r="F23" t="s">
+        <v>138</v>
+      </c>
+      <c r="G23" t="s">
+        <v>102</v>
+      </c>
+      <c r="H23" t="s">
+        <v>99</v>
+      </c>
+      <c r="I23" t="s">
+        <v>111</v>
+      </c>
+      <c r="J23">
+        <v>0.75</v>
+      </c>
+      <c r="K23">
+        <v>0.75</v>
+      </c>
+      <c r="L23">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="M23">
+        <v>3000.1</v>
+      </c>
+      <c r="N23" s="3">
+        <v>10000</v>
+      </c>
+      <c r="O23">
+        <v>0</v>
+      </c>
+      <c r="P23">
+        <v>0.1</v>
+      </c>
+      <c r="Q23" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="R23" t="s">
+        <v>101</v>
+      </c>
+      <c r="S23">
+        <v>0</v>
+      </c>
+      <c r="T23">
+        <v>100</v>
+      </c>
+      <c r="U23">
+        <v>5000</v>
+      </c>
+      <c r="V23">
+        <v>100</v>
+      </c>
+      <c r="W23">
+        <v>1000</v>
+      </c>
+      <c r="X23">
+        <v>0</v>
+      </c>
+      <c r="Y23">
+        <v>0</v>
+      </c>
+      <c r="Z23">
+        <v>0.04</v>
+      </c>
+      <c r="AA23">
+        <v>0.42</v>
+      </c>
+      <c r="AB23">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="AC23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="E24" s="7">
+        <v>1.2</v>
+      </c>
+      <c r="F24" t="s">
+        <v>139</v>
+      </c>
+      <c r="G24" t="s">
+        <v>140</v>
+      </c>
+      <c r="H24" t="s">
+        <v>106</v>
+      </c>
+      <c r="I24" t="s">
+        <v>111</v>
+      </c>
+      <c r="J24">
+        <v>0.75</v>
+      </c>
+      <c r="K24">
+        <v>0.75</v>
+      </c>
+      <c r="L24">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="M24">
+        <v>3000.1</v>
+      </c>
+      <c r="N24" s="3">
+        <v>10000</v>
+      </c>
+      <c r="O24">
+        <v>0</v>
+      </c>
+      <c r="P24">
+        <v>0.1</v>
+      </c>
+      <c r="Q24" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="R24" t="s">
+        <v>101</v>
+      </c>
+      <c r="S24">
+        <v>0</v>
+      </c>
+      <c r="T24">
+        <v>100</v>
+      </c>
+      <c r="U24">
+        <v>5000</v>
+      </c>
+      <c r="V24">
+        <v>100</v>
+      </c>
+      <c r="W24">
+        <v>1000</v>
+      </c>
+      <c r="X24">
+        <v>0</v>
+      </c>
+      <c r="Y24">
+        <v>0</v>
+      </c>
+      <c r="Z24">
+        <v>0.04</v>
+      </c>
+      <c r="AA24">
+        <v>0.42</v>
+      </c>
+      <c r="AB24">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="AC24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="E25" s="7">
+        <v>1.5</v>
+      </c>
+      <c r="F25" t="s">
+        <v>141</v>
+      </c>
+      <c r="G25" t="s">
+        <v>142</v>
+      </c>
+      <c r="H25" t="s">
+        <v>106</v>
+      </c>
+      <c r="I25" t="s">
+        <v>111</v>
+      </c>
+      <c r="J25">
+        <v>0.75</v>
+      </c>
+      <c r="K25">
+        <v>0.75</v>
+      </c>
+      <c r="L25">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="M25">
+        <v>4000.1</v>
+      </c>
+      <c r="N25" s="3">
+        <v>10000</v>
+      </c>
+      <c r="O25">
+        <v>0</v>
+      </c>
+      <c r="P25">
+        <v>0.1</v>
+      </c>
+      <c r="Q25" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="R25" t="s">
+        <v>101</v>
+      </c>
+      <c r="S25">
+        <v>0</v>
+      </c>
+      <c r="T25">
+        <v>100</v>
+      </c>
+      <c r="U25">
+        <v>5000</v>
+      </c>
+      <c r="V25">
+        <v>100</v>
+      </c>
+      <c r="W25">
+        <v>1000</v>
+      </c>
+      <c r="X25">
+        <v>0</v>
+      </c>
+      <c r="Y25">
+        <v>0</v>
+      </c>
+      <c r="Z25">
+        <v>0.04</v>
+      </c>
+      <c r="AA25">
+        <v>0.42</v>
+      </c>
+      <c r="AB25">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="AC25">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>